<commit_message>
Paar refactorings, en wat commentaar toegevoegd.
</commit_message>
<xml_diff>
--- a/Financieel_rekenwerk_V3.xlsx
+++ b/Financieel_rekenwerk_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projecten\FsFinancieelExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C7B044-F454-4D88-9204-E1C1EBED02E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6B3D59-3271-4DE6-9A33-C1CD2865BF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{80C5C2A5-8FFD-49F2-A478-6BCA3C7B4B74}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Rente</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>Eigen C# projectje, met voorzet van CoPilot</t>
+  </si>
+  <si>
+    <t>4 + (5/12)</t>
+  </si>
+  <si>
+    <t>hoofdsom</t>
+  </si>
+  <si>
+    <t>looptijd</t>
   </si>
 </sst>
 </file>
@@ -350,7 +359,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -372,6 +381,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Berekening" xfId="2" builtinId="22"/>
@@ -950,10 +961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7AF0AE-354E-456E-897C-228CAE9D0A1D}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1197,6 +1208,38 @@
         <v>40</v>
       </c>
     </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>5500</v>
+      </c>
+      <c r="B52" s="20">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="C52">
+        <f>4+(5/12)</f>
+        <v>4.416666666666667</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <f>A52*(1 + B52)^C52</f>
+        <v>6484.8659159352792</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" display="https://economiecompactonline.nl/beco/vwo/interest_contantewaarde_renten.php" xr:uid="{6E09A0F6-8E23-461E-B4DC-016207CEE69A}"/>

</xml_diff>

<commit_message>
Aantal maanden toegevoegd aan berekening (dus aantal jaren + [aantal maanden/12.0] = aangtaltijdeeenheden)
</commit_message>
<xml_diff>
--- a/Financieel_rekenwerk_V3.xlsx
+++ b/Financieel_rekenwerk_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projecten\FsFinancieelExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6B3D59-3271-4DE6-9A33-C1CD2865BF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DA7BDC-0B76-4E46-A59A-D976D0545C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{80C5C2A5-8FFD-49F2-A478-6BCA3C7B4B74}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Rente</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>looptijd</t>
+  </si>
+  <si>
+    <t>Basisboek wiskunde en financiële rekenkunde, voorbeeld 4.8 p. 153</t>
   </si>
 </sst>
 </file>
@@ -961,10 +964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7AF0AE-354E-456E-897C-228CAE9D0A1D}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1208,6 +1211,11 @@
         <v>40</v>
       </c>
     </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>43</v>
@@ -1238,6 +1246,23 @@
       <c r="A53">
         <f>A52*(1 + B52)^C52</f>
         <v>6484.8659159352792</v>
+      </c>
+      <c r="B53" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A53)</f>
+        <v>=A52*(1 + B52)^C52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="8">
+        <f>FV(B52,C52,0,-A52,0)</f>
+        <v>6484.8659159352792</v>
+      </c>
+      <c r="B55" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A55)</f>
+        <v>=TW(B52;C52;0;-A52;0)</v>
+      </c>
+      <c r="D55" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eerste unit test toegevoegd voor TW (met e-macht)
</commit_message>
<xml_diff>
--- a/Financieel_rekenwerk_V3.xlsx
+++ b/Financieel_rekenwerk_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projecten\FsFinancieelExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DA7BDC-0B76-4E46-A59A-D976D0545C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9EFBEA-4B22-4A75-B998-7A86E5C05C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{80C5C2A5-8FFD-49F2-A478-6BCA3C7B4B74}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t>Rente</t>
   </si>
@@ -213,14 +213,24 @@
   <si>
     <t>Basisboek wiskunde en financiële rekenkunde, voorbeeld 4.8 p. 153</t>
   </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>Eerste unit test (met e^(r.t)</t>
+  </si>
+  <si>
+    <t>looptijd in jaren</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;€&quot;\ #,##0.00;[Red]&quot;€&quot;\ \-#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_ [$€-413]\ * #,##0.00_ ;_ [$€-413]\ * \-#,##0.00_ ;_ [$€-413]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -362,7 +372,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -386,6 +396,7 @@
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Berekening" xfId="2" builtinId="22"/>
@@ -964,10 +975,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7AF0AE-354E-456E-897C-228CAE9D0A1D}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1265,6 +1276,43 @@
         <v>33</v>
       </c>
     </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>1000</v>
+      </c>
+      <c r="B59">
+        <v>10</v>
+      </c>
+      <c r="C59" s="9">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="21">
+        <f>ROUND(A59*EXP(B59*C59),2)</f>
+        <v>1648.72</v>
+      </c>
+      <c r="B60" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(A60)</f>
+        <v>=AFRONDEN(A59*EXP(B59*C59);2)</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" display="https://economiecompactonline.nl/beco/vwo/interest_contantewaarde_renten.php" xr:uid="{6E09A0F6-8E23-461E-B4DC-016207CEE69A}"/>

</xml_diff>

<commit_message>
Paar kleine wijzigingen in berekening TW. 2 Unit teststoegevoegd.
</commit_message>
<xml_diff>
--- a/Financieel_rekenwerk_V3.xlsx
+++ b/Financieel_rekenwerk_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projecten\FsFinancieelExpert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9EFBEA-4B22-4A75-B998-7A86E5C05C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8576A955-64AE-465A-B296-D5A06E51C741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{80C5C2A5-8FFD-49F2-A478-6BCA3C7B4B74}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>Rente</t>
   </si>
@@ -221,6 +221,18 @@
   </si>
   <si>
     <t>looptijd in jaren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        /// TW(0.05;2;-1000; 0; 0) = € 1102.50. [0 = Postnumerando]</t>
+  </si>
+  <si>
+    <t>Test de berekening van de toekomstige waarde met enkel een hoofdsom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Excel is dit :   </t>
+  </si>
+  <si>
+    <t>achteraf, zonder peridieke betalingen.</t>
   </si>
 </sst>
 </file>
@@ -975,10 +987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E7AF0AE-354E-456E-897C-228CAE9D0A1D}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1313,6 +1325,54 @@
         <v>=AFRONDEN(A59*EXP(B59*C59);2)</v>
       </c>
     </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>-1000</v>
+      </c>
+      <c r="B68" s="20">
+        <v>0.05</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="8">
+        <f>FV(B68, C68, 0, A68, 0)</f>
+        <v>1102.5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" display="https://economiecompactonline.nl/beco/vwo/interest_contantewaarde_renten.php" xr:uid="{6E09A0F6-8E23-461E-B4DC-016207CEE69A}"/>

</xml_diff>